<commit_message>
First commit , admin data removed
</commit_message>
<xml_diff>
--- a/TestData/Staging/Web_POS/Billing/billing_test_data.xlsx
+++ b/TestData/Staging/Web_POS/Billing/billing_test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Calc"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Staging\Web_POS\Billing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\zwing-qa-automation\TestData\Staging\Web_POS\Billing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -393,7 +393,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -407,11 +407,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -469,25 +464,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border/>
-    <border>
-      <left>
-        <color indexed="64"/>
-      </left>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-      <diagonal>
-        <color indexed="64"/>
-      </diagonal>
-    </border>
     <border>
       <right style="medium">
         <color rgb="FF2B579A"/>
@@ -500,11 +478,11 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -516,15 +494,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -536,11 +512,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -737,11 +713,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="R1">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="I22">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.542969" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.542969" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.68" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.28" style="3" customWidth="1"/>
@@ -762,7 +738,7 @@
     <col min="24" max="25" width="12.68" style="3" customWidth="1"/>
     <col min="26" max="26" width="22.85" style="3" customWidth="1"/>
     <col min="27" max="28" width="12.68" style="3" customWidth="1"/>
-    <col min="29" max="29" width="18.5625" style="5" customWidth="1"/>
+    <col min="29" max="29" width="18.5625" style="3" customWidth="1"/>
     <col min="30" max="1025" width="12.68" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -770,19 +746,19 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -851,7 +827,7 @@
       <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -859,7 +835,7 @@
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -874,10 +850,10 @@
       <c r="F2" s="3">
         <v>123456</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -928,7 +904,7 @@
       <c r="Z2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="AC2" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -936,7 +912,7 @@
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -951,10 +927,10 @@
       <c r="F3" s="3">
         <v>123456</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -1008,39 +984,39 @@
       <c r="Z3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AC3" s="3">
         <v>9874563212</v>
       </c>
     </row>
     <row r="4" ht="33" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>123456</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="10">
-        <v>123456</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="F4" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="9" t="s">
         <v>42</v>
       </c>
       <c r="K4" s="1">
@@ -1055,11 +1031,11 @@
       <c r="N4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12" t="s">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="10" t="s">
         <v>45</v>
       </c>
       <c r="R4" s="4" t="s">
@@ -1089,40 +1065,40 @@
       <c r="Z4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AA4" s="9"/>
-      <c r="AC4" s="5">
+      <c r="AA4" s="7"/>
+      <c r="AC4" s="3">
         <v>9874563212</v>
       </c>
     </row>
     <row r="5" ht="34.8" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>123456</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="10">
-        <v>123456</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="9">
         <v>1</v>
       </c>
       <c r="K5" s="1">
@@ -1137,11 +1113,11 @@
       <c r="N5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="10" t="s">
         <v>45</v>
       </c>
       <c r="R5" s="4" t="s">
@@ -1171,8 +1147,8 @@
       <c r="Z5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AA5" s="9"/>
-      <c r="AC5" s="5">
+      <c r="AA5" s="7"/>
+      <c r="AC5" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1180,34 +1156,34 @@
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>123456</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="11">
         <v>1</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="11">
         <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1219,13 +1195,13 @@
       <c r="N6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="12">
         <v>45384</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R6" s="4" t="s">
@@ -1255,7 +1231,7 @@
       <c r="Z6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC6" s="5">
+      <c r="AC6" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1263,34 +1239,34 @@
       <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>123456</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="11">
         <v>1</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="11">
         <v>1</v>
       </c>
       <c r="L7" s="4" t="s">
@@ -1302,13 +1278,13 @@
       <c r="N7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="12">
         <v>45384</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R7" s="2">
@@ -1338,7 +1314,7 @@
       <c r="Z7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC7" s="5">
+      <c r="AC7" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1346,34 +1322,34 @@
       <c r="A8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>123456</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="F8" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="11">
         <v>1</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="11">
         <v>1</v>
       </c>
       <c r="L8" s="4" t="s">
@@ -1385,13 +1361,13 @@
       <c r="N8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="12">
         <v>45384</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R8" s="2">
@@ -1421,7 +1397,7 @@
       <c r="Z8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC8" s="5">
+      <c r="AC8" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1429,31 +1405,31 @@
       <c r="A9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>123456</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="10">
-        <v>123456</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="9">
         <v>1</v>
       </c>
       <c r="K9" s="1">
@@ -1468,11 +1444,11 @@
       <c r="N9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12" t="s">
+      <c r="O9" s="10"/>
+      <c r="P9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="Q9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="R9" s="4" t="s">
@@ -1502,7 +1478,7 @@
       <c r="Z9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC9" s="5">
+      <c r="AC9" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1510,31 +1486,31 @@
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>123456</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="10">
-        <v>123456</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="9">
         <v>1</v>
       </c>
       <c r="K10" s="1">
@@ -1549,11 +1525,11 @@
       <c r="N10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12" t="s">
+      <c r="O10" s="10"/>
+      <c r="P10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" s="12" t="s">
+      <c r="Q10" s="10" t="s">
         <v>45</v>
       </c>
       <c r="R10" s="4" t="s">
@@ -1583,7 +1559,7 @@
       <c r="Z10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC10" s="5">
+      <c r="AC10" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1591,34 +1567,34 @@
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>123456</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="11">
         <v>1</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="11">
         <v>1</v>
       </c>
       <c r="L11" s="4" t="s">
@@ -1630,13 +1606,13 @@
       <c r="N11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="12">
         <v>45384</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R11" s="2">
@@ -1666,7 +1642,7 @@
       <c r="Z11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC11" s="5">
+      <c r="AC11" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1674,34 +1650,34 @@
       <c r="A12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>123456</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="11">
         <v>1</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="11">
         <v>1</v>
       </c>
       <c r="L12" s="4" t="s">
@@ -1713,13 +1689,13 @@
       <c r="N12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="12">
         <v>45384</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R12" s="2">
@@ -1749,7 +1725,7 @@
       <c r="Z12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC12" s="5">
+      <c r="AC12" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1757,34 +1733,34 @@
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>123456</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="11">
         <v>1</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="11">
         <v>1</v>
       </c>
       <c r="L13" s="4" t="s">
@@ -1796,13 +1772,13 @@
       <c r="N13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="12">
         <v>45384</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q13" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R13" s="2">
@@ -1832,7 +1808,7 @@
       <c r="Z13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC13" s="5">
+      <c r="AC13" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1840,34 +1816,34 @@
       <c r="A14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>123456</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F14" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="11">
         <v>1</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="11">
         <v>1</v>
       </c>
       <c r="L14" s="4" t="s">
@@ -1879,13 +1855,13 @@
       <c r="N14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="12">
         <v>45384</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="P14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q14" s="14" t="s">
+      <c r="Q14" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R14" s="2">
@@ -1915,7 +1891,7 @@
       <c r="Z14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC14" s="5">
+      <c r="AC14" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -1923,34 +1899,34 @@
       <c r="A15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="13">
         <v>123456</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="F15" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="11">
         <v>1</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="11">
         <v>1</v>
       </c>
       <c r="L15" s="4" t="s">
@@ -1962,13 +1938,13 @@
       <c r="N15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="12">
         <v>45384</v>
       </c>
-      <c r="P15" s="14" t="s">
+      <c r="P15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R15" s="2">
@@ -1998,33 +1974,33 @@
       <c r="Z15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC15" s="5">
+      <c r="AC15" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1">
+    <row r="16" s="1" customFormat="1" ht="14.25">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="8">
         <v>123456</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="10">
-        <v>123456</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="F16" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2045,11 +2021,11 @@
       <c r="N16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12" t="s">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q16" s="12" t="s">
+      <c r="Q16" s="10" t="s">
         <v>45</v>
       </c>
       <c r="R16" s="4" t="s">
@@ -2079,512 +2055,512 @@
       <c r="Z16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AC16" s="5">
+      <c r="AC16" s="3">
         <v>9874563212</v>
       </c>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="12"/>
-      <c r="AJ16" s="16"/>
-      <c r="AK16" s="10"/>
-      <c r="AL16" s="10"/>
-      <c r="AM16" s="10"/>
-      <c r="AN16" s="10"/>
-      <c r="AW16" s="12"/>
-      <c r="AX16" s="12"/>
-      <c r="AY16" s="12"/>
-      <c r="BA16" s="16"/>
-      <c r="BB16" s="10"/>
-      <c r="BC16" s="10"/>
-      <c r="BD16" s="10"/>
-      <c r="BE16" s="10"/>
-      <c r="BN16" s="12"/>
-      <c r="BO16" s="12"/>
-      <c r="BP16" s="12"/>
-      <c r="BR16" s="16"/>
-      <c r="BS16" s="10"/>
-      <c r="BT16" s="10"/>
-      <c r="BU16" s="10"/>
-      <c r="BV16" s="10"/>
-      <c r="CE16" s="12"/>
-      <c r="CF16" s="12"/>
-      <c r="CG16" s="12"/>
-      <c r="CI16" s="16"/>
-      <c r="CJ16" s="10"/>
-      <c r="CK16" s="10"/>
-      <c r="CL16" s="10"/>
-      <c r="CM16" s="10"/>
-      <c r="CV16" s="12"/>
-      <c r="CW16" s="12"/>
-      <c r="CX16" s="12"/>
-      <c r="CZ16" s="16"/>
-      <c r="DA16" s="10"/>
-      <c r="DB16" s="10"/>
-      <c r="DC16" s="10"/>
-      <c r="DD16" s="10"/>
-      <c r="DM16" s="12"/>
-      <c r="DN16" s="12"/>
-      <c r="DO16" s="12"/>
-      <c r="DQ16" s="16"/>
-      <c r="DR16" s="10"/>
-      <c r="DS16" s="10"/>
-      <c r="DT16" s="10"/>
-      <c r="DU16" s="10"/>
-      <c r="ED16" s="12"/>
-      <c r="EE16" s="12"/>
-      <c r="EF16" s="12"/>
-      <c r="EH16" s="16"/>
-      <c r="EI16" s="10"/>
-      <c r="EJ16" s="10"/>
-      <c r="EK16" s="10"/>
-      <c r="EL16" s="10"/>
-      <c r="EU16" s="12"/>
-      <c r="EV16" s="12"/>
-      <c r="EW16" s="12"/>
-      <c r="EY16" s="16"/>
-      <c r="EZ16" s="10"/>
-      <c r="FA16" s="10"/>
-      <c r="FB16" s="10"/>
-      <c r="FC16" s="10"/>
-      <c r="FL16" s="12"/>
-      <c r="FM16" s="12"/>
-      <c r="FN16" s="12"/>
-      <c r="FP16" s="16"/>
-      <c r="FQ16" s="10"/>
-      <c r="FR16" s="10"/>
-      <c r="FS16" s="10"/>
-      <c r="FT16" s="10"/>
-      <c r="GC16" s="12"/>
-      <c r="GD16" s="12"/>
-      <c r="GE16" s="12"/>
-      <c r="GG16" s="16"/>
-      <c r="GH16" s="10"/>
-      <c r="GI16" s="10"/>
-      <c r="GJ16" s="10"/>
-      <c r="GK16" s="10"/>
-      <c r="GT16" s="12"/>
-      <c r="GU16" s="12"/>
-      <c r="GV16" s="12"/>
-      <c r="GX16" s="16"/>
-      <c r="GY16" s="10"/>
-      <c r="GZ16" s="10"/>
-      <c r="HA16" s="10"/>
-      <c r="HB16" s="10"/>
-      <c r="HK16" s="12"/>
-      <c r="HL16" s="12"/>
-      <c r="HM16" s="12"/>
-      <c r="HO16" s="16"/>
-      <c r="HP16" s="10"/>
-      <c r="HQ16" s="10"/>
-      <c r="HR16" s="10"/>
-      <c r="HS16" s="10"/>
-      <c r="IB16" s="12"/>
-      <c r="IC16" s="12"/>
-      <c r="ID16" s="12"/>
-      <c r="IF16" s="16"/>
-      <c r="IG16" s="10"/>
-      <c r="IH16" s="10"/>
-      <c r="II16" s="10"/>
-      <c r="IJ16" s="10"/>
-      <c r="IS16" s="12"/>
-      <c r="IT16" s="12"/>
-      <c r="IU16" s="12"/>
-      <c r="IW16" s="16"/>
-      <c r="IX16" s="10"/>
-      <c r="IY16" s="10"/>
-      <c r="IZ16" s="10"/>
-      <c r="JA16" s="10"/>
-      <c r="JJ16" s="12"/>
-      <c r="JK16" s="12"/>
-      <c r="JL16" s="12"/>
-      <c r="JN16" s="16"/>
-      <c r="JO16" s="10"/>
-      <c r="JP16" s="10"/>
-      <c r="JQ16" s="10"/>
-      <c r="JR16" s="10"/>
-      <c r="KA16" s="12"/>
-      <c r="KB16" s="12"/>
-      <c r="KC16" s="12"/>
-      <c r="KE16" s="16"/>
-      <c r="KF16" s="10"/>
-      <c r="KG16" s="10"/>
-      <c r="KH16" s="10"/>
-      <c r="KI16" s="10"/>
-      <c r="KR16" s="12"/>
-      <c r="KS16" s="12"/>
-      <c r="KT16" s="12"/>
-      <c r="KV16" s="16"/>
-      <c r="KW16" s="10"/>
-      <c r="KX16" s="10"/>
-      <c r="KY16" s="10"/>
-      <c r="KZ16" s="10"/>
-      <c r="LI16" s="12"/>
-      <c r="LJ16" s="12"/>
-      <c r="LK16" s="12"/>
-      <c r="LM16" s="16"/>
-      <c r="LN16" s="10"/>
-      <c r="LO16" s="10"/>
-      <c r="LP16" s="10"/>
-      <c r="LQ16" s="10"/>
-      <c r="LZ16" s="12"/>
-      <c r="MA16" s="12"/>
-      <c r="MB16" s="12"/>
-      <c r="MD16" s="16"/>
-      <c r="ME16" s="10"/>
-      <c r="MF16" s="10"/>
-      <c r="MG16" s="10"/>
-      <c r="MH16" s="10"/>
-      <c r="MQ16" s="12"/>
-      <c r="MR16" s="12"/>
-      <c r="MS16" s="12"/>
-      <c r="MU16" s="16"/>
-      <c r="MV16" s="10"/>
-      <c r="MW16" s="10"/>
-      <c r="MX16" s="10"/>
-      <c r="MY16" s="10"/>
-      <c r="NH16" s="12"/>
-      <c r="NI16" s="12"/>
-      <c r="NJ16" s="12"/>
-      <c r="NL16" s="16"/>
-      <c r="NM16" s="10"/>
-      <c r="NN16" s="10"/>
-      <c r="NO16" s="10"/>
-      <c r="NP16" s="10"/>
-      <c r="NY16" s="12"/>
-      <c r="NZ16" s="12"/>
-      <c r="OA16" s="12"/>
-      <c r="OC16" s="16"/>
-      <c r="OD16" s="10"/>
-      <c r="OE16" s="10"/>
-      <c r="OF16" s="10"/>
-      <c r="OG16" s="10"/>
-      <c r="OP16" s="12"/>
-      <c r="OQ16" s="12"/>
-      <c r="OR16" s="12"/>
-      <c r="OT16" s="16"/>
-      <c r="OU16" s="10"/>
-      <c r="OV16" s="10"/>
-      <c r="OW16" s="10"/>
-      <c r="OX16" s="10"/>
-      <c r="PG16" s="12"/>
-      <c r="PH16" s="12"/>
-      <c r="PI16" s="12"/>
-      <c r="PK16" s="16"/>
-      <c r="PL16" s="10"/>
-      <c r="PM16" s="10"/>
-      <c r="PN16" s="10"/>
-      <c r="PO16" s="10"/>
-      <c r="PX16" s="12"/>
-      <c r="PY16" s="12"/>
-      <c r="PZ16" s="12"/>
-      <c r="QB16" s="16"/>
-      <c r="QC16" s="10"/>
-      <c r="QD16" s="10"/>
-      <c r="QE16" s="10"/>
-      <c r="QF16" s="10"/>
-      <c r="QO16" s="12"/>
-      <c r="QP16" s="12"/>
-      <c r="QQ16" s="12"/>
-      <c r="QS16" s="16"/>
-      <c r="QT16" s="10"/>
-      <c r="QU16" s="10"/>
-      <c r="QV16" s="10"/>
-      <c r="QW16" s="10"/>
-      <c r="RF16" s="12"/>
-      <c r="RG16" s="12"/>
-      <c r="RH16" s="12"/>
-      <c r="RJ16" s="16"/>
-      <c r="RK16" s="10"/>
-      <c r="RL16" s="10"/>
-      <c r="RM16" s="10"/>
-      <c r="RN16" s="10"/>
-      <c r="RW16" s="12"/>
-      <c r="RX16" s="12"/>
-      <c r="RY16" s="12"/>
-      <c r="SA16" s="16"/>
-      <c r="SB16" s="10"/>
-      <c r="SC16" s="10"/>
-      <c r="SD16" s="10"/>
-      <c r="SE16" s="10"/>
-      <c r="SN16" s="12"/>
-      <c r="SO16" s="12"/>
-      <c r="SP16" s="12"/>
-      <c r="SR16" s="16"/>
-      <c r="SS16" s="10"/>
-      <c r="ST16" s="10"/>
-      <c r="SU16" s="10"/>
-      <c r="SV16" s="10"/>
-      <c r="TE16" s="12"/>
-      <c r="TF16" s="12"/>
-      <c r="TG16" s="12"/>
-      <c r="TI16" s="16"/>
-      <c r="TJ16" s="10"/>
-      <c r="TK16" s="10"/>
-      <c r="TL16" s="10"/>
-      <c r="TM16" s="10"/>
-      <c r="TV16" s="12"/>
-      <c r="TW16" s="12"/>
-      <c r="TX16" s="12"/>
-      <c r="TZ16" s="16"/>
-      <c r="UA16" s="10"/>
-      <c r="UB16" s="10"/>
-      <c r="UC16" s="10"/>
-      <c r="UD16" s="10"/>
-      <c r="UM16" s="12"/>
-      <c r="UN16" s="12"/>
-      <c r="UO16" s="12"/>
-      <c r="UQ16" s="16"/>
-      <c r="UR16" s="10"/>
-      <c r="US16" s="10"/>
-      <c r="UT16" s="10"/>
-      <c r="UU16" s="10"/>
-      <c r="VD16" s="12"/>
-      <c r="VE16" s="12"/>
-      <c r="VF16" s="12"/>
-      <c r="VH16" s="16"/>
-      <c r="VI16" s="10"/>
-      <c r="VJ16" s="10"/>
-      <c r="VK16" s="10"/>
-      <c r="VL16" s="10"/>
-      <c r="VU16" s="12"/>
-      <c r="VV16" s="12"/>
-      <c r="VW16" s="12"/>
-      <c r="VY16" s="16"/>
-      <c r="VZ16" s="10"/>
-      <c r="WA16" s="10"/>
-      <c r="WB16" s="10"/>
-      <c r="WC16" s="10"/>
-      <c r="WL16" s="12"/>
-      <c r="WM16" s="12"/>
-      <c r="WN16" s="12"/>
-      <c r="WP16" s="16"/>
-      <c r="WQ16" s="10"/>
-      <c r="WR16" s="10"/>
-      <c r="WS16" s="10"/>
-      <c r="WT16" s="10"/>
-      <c r="XC16" s="12"/>
-      <c r="XD16" s="12"/>
-      <c r="XE16" s="12"/>
-      <c r="XG16" s="16"/>
-      <c r="XH16" s="10"/>
-      <c r="XI16" s="10"/>
-      <c r="XJ16" s="10"/>
-      <c r="XK16" s="10"/>
-      <c r="XT16" s="12"/>
-      <c r="XU16" s="12"/>
-      <c r="XV16" s="12"/>
-      <c r="XX16" s="16"/>
-      <c r="XY16" s="10"/>
-      <c r="XZ16" s="10"/>
-      <c r="YA16" s="10"/>
-      <c r="YB16" s="10"/>
-      <c r="YK16" s="12"/>
-      <c r="YL16" s="12"/>
-      <c r="YM16" s="12"/>
-      <c r="YO16" s="16"/>
-      <c r="YP16" s="10"/>
-      <c r="YQ16" s="10"/>
-      <c r="YR16" s="10"/>
-      <c r="YS16" s="10"/>
-      <c r="ZB16" s="12"/>
-      <c r="ZC16" s="12"/>
-      <c r="ZD16" s="12"/>
-      <c r="ZF16" s="16"/>
-      <c r="ZG16" s="10"/>
-      <c r="ZH16" s="10"/>
-      <c r="ZI16" s="10"/>
-      <c r="ZJ16" s="10"/>
-      <c r="ZS16" s="12"/>
-      <c r="ZT16" s="12"/>
-      <c r="ZU16" s="12"/>
-      <c r="ZW16" s="16"/>
-      <c r="ZX16" s="10"/>
-      <c r="ZY16" s="10"/>
-      <c r="ZZ16" s="10"/>
-      <c r="AAA16" s="10"/>
-      <c r="AAJ16" s="12"/>
-      <c r="AAK16" s="12"/>
-      <c r="AAL16" s="12"/>
-      <c r="AAN16" s="16"/>
-      <c r="AAO16" s="10"/>
-      <c r="AAP16" s="10"/>
-      <c r="AAQ16" s="10"/>
-      <c r="AAR16" s="10"/>
-      <c r="ABA16" s="12"/>
-      <c r="ABB16" s="12"/>
-      <c r="ABC16" s="12"/>
-      <c r="ABE16" s="16"/>
-      <c r="ABF16" s="10"/>
-      <c r="ABG16" s="10"/>
-      <c r="ABH16" s="10"/>
-      <c r="ABI16" s="10"/>
-      <c r="ABR16" s="12"/>
-      <c r="ABS16" s="12"/>
-      <c r="ABT16" s="12"/>
-      <c r="ABV16" s="16"/>
-      <c r="ABW16" s="10"/>
-      <c r="ABX16" s="10"/>
-      <c r="ABY16" s="10"/>
-      <c r="ABZ16" s="10"/>
-      <c r="ACI16" s="12"/>
-      <c r="ACJ16" s="12"/>
-      <c r="ACK16" s="12"/>
-      <c r="ACM16" s="16"/>
-      <c r="ACN16" s="10"/>
-      <c r="ACO16" s="10"/>
-      <c r="ACP16" s="10"/>
-      <c r="ACQ16" s="10"/>
-      <c r="ACZ16" s="12"/>
-      <c r="ADA16" s="12"/>
-      <c r="ADB16" s="12"/>
-      <c r="ADD16" s="16"/>
-      <c r="ADE16" s="10"/>
-      <c r="ADF16" s="10"/>
-      <c r="ADG16" s="10"/>
-      <c r="ADH16" s="10"/>
-      <c r="ADQ16" s="12"/>
-      <c r="ADR16" s="12"/>
-      <c r="ADS16" s="12"/>
-      <c r="ADU16" s="16"/>
-      <c r="ADV16" s="10"/>
-      <c r="ADW16" s="10"/>
-      <c r="ADX16" s="10"/>
-      <c r="ADY16" s="10"/>
-      <c r="AEH16" s="12"/>
-      <c r="AEI16" s="12"/>
-      <c r="AEJ16" s="12"/>
-      <c r="AEL16" s="16"/>
-      <c r="AEM16" s="10"/>
-      <c r="AEN16" s="10"/>
-      <c r="AEO16" s="10"/>
-      <c r="AEP16" s="10"/>
-      <c r="AEY16" s="12"/>
-      <c r="AEZ16" s="12"/>
-      <c r="AFA16" s="12"/>
-      <c r="AFC16" s="16"/>
-      <c r="AFD16" s="10"/>
-      <c r="AFE16" s="10"/>
-      <c r="AFF16" s="10"/>
-      <c r="AFG16" s="10"/>
-      <c r="AFP16" s="12"/>
-      <c r="AFQ16" s="12"/>
-      <c r="AFR16" s="12"/>
-      <c r="AFT16" s="16"/>
-      <c r="AFU16" s="10"/>
-      <c r="AFV16" s="10"/>
-      <c r="AFW16" s="10"/>
-      <c r="AFX16" s="10"/>
-      <c r="AGG16" s="12"/>
-      <c r="AGH16" s="12"/>
-      <c r="AGI16" s="12"/>
-      <c r="AGK16" s="16"/>
-      <c r="AGL16" s="10"/>
-      <c r="AGM16" s="10"/>
-      <c r="AGN16" s="10"/>
-      <c r="AGO16" s="10"/>
-      <c r="AGX16" s="12"/>
-      <c r="AGY16" s="12"/>
-      <c r="AGZ16" s="12"/>
-      <c r="AHB16" s="16"/>
-      <c r="AHC16" s="10"/>
-      <c r="AHD16" s="10"/>
-      <c r="AHE16" s="10"/>
-      <c r="AHF16" s="10"/>
-      <c r="AHO16" s="12"/>
-      <c r="AHP16" s="12"/>
-      <c r="AHQ16" s="12"/>
-      <c r="AHS16" s="16"/>
-      <c r="AHT16" s="10"/>
-      <c r="AHU16" s="10"/>
-      <c r="AHV16" s="10"/>
-      <c r="AHW16" s="10"/>
-      <c r="AIF16" s="12"/>
-      <c r="AIG16" s="12"/>
-      <c r="AIH16" s="12"/>
-      <c r="AIJ16" s="16"/>
-      <c r="AIK16" s="10"/>
-      <c r="AIL16" s="10"/>
-      <c r="AIM16" s="10"/>
-      <c r="AIN16" s="10"/>
-      <c r="AIW16" s="12"/>
-      <c r="AIX16" s="12"/>
-      <c r="AIY16" s="12"/>
-      <c r="AJA16" s="16"/>
-      <c r="AJB16" s="10"/>
-      <c r="AJC16" s="10"/>
-      <c r="AJD16" s="10"/>
-      <c r="AJE16" s="10"/>
-      <c r="AJN16" s="12"/>
-      <c r="AJO16" s="12"/>
-      <c r="AJP16" s="12"/>
-      <c r="AJR16" s="16"/>
-      <c r="AJS16" s="10"/>
-      <c r="AJT16" s="10"/>
-      <c r="AJU16" s="10"/>
-      <c r="AJV16" s="10"/>
-      <c r="AKE16" s="12"/>
-      <c r="AKF16" s="12"/>
-      <c r="AKG16" s="12"/>
-      <c r="AKI16" s="16"/>
-      <c r="AKJ16" s="10"/>
-      <c r="AKK16" s="10"/>
-      <c r="AKL16" s="10"/>
-      <c r="AKM16" s="10"/>
-      <c r="AKV16" s="12"/>
-      <c r="AKW16" s="12"/>
-      <c r="AKX16" s="12"/>
-      <c r="AKZ16" s="16"/>
-      <c r="ALA16" s="10"/>
-      <c r="ALB16" s="10"/>
-      <c r="ALC16" s="10"/>
-      <c r="ALD16" s="10"/>
-      <c r="ALM16" s="12"/>
-      <c r="ALN16" s="12"/>
-      <c r="ALO16" s="12"/>
-      <c r="ALQ16" s="16"/>
-      <c r="ALR16" s="10"/>
-      <c r="ALS16" s="10"/>
-      <c r="ALT16" s="10"/>
-      <c r="ALU16" s="10"/>
-      <c r="AMD16" s="12"/>
-      <c r="AME16" s="12"/>
-      <c r="AMF16" s="12"/>
-      <c r="AMH16" s="16"/>
-      <c r="AMI16" s="10"/>
-      <c r="AMJ16" s="10"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="10"/>
+      <c r="AJ16" s="14"/>
+      <c r="AK16" s="8"/>
+      <c r="AL16" s="8"/>
+      <c r="AM16" s="8"/>
+      <c r="AN16" s="8"/>
+      <c r="AW16" s="10"/>
+      <c r="AX16" s="10"/>
+      <c r="AY16" s="10"/>
+      <c r="BA16" s="14"/>
+      <c r="BB16" s="8"/>
+      <c r="BC16" s="8"/>
+      <c r="BD16" s="8"/>
+      <c r="BE16" s="8"/>
+      <c r="BN16" s="10"/>
+      <c r="BO16" s="10"/>
+      <c r="BP16" s="10"/>
+      <c r="BR16" s="14"/>
+      <c r="BS16" s="8"/>
+      <c r="BT16" s="8"/>
+      <c r="BU16" s="8"/>
+      <c r="BV16" s="8"/>
+      <c r="CE16" s="10"/>
+      <c r="CF16" s="10"/>
+      <c r="CG16" s="10"/>
+      <c r="CI16" s="14"/>
+      <c r="CJ16" s="8"/>
+      <c r="CK16" s="8"/>
+      <c r="CL16" s="8"/>
+      <c r="CM16" s="8"/>
+      <c r="CV16" s="10"/>
+      <c r="CW16" s="10"/>
+      <c r="CX16" s="10"/>
+      <c r="CZ16" s="14"/>
+      <c r="DA16" s="8"/>
+      <c r="DB16" s="8"/>
+      <c r="DC16" s="8"/>
+      <c r="DD16" s="8"/>
+      <c r="DM16" s="10"/>
+      <c r="DN16" s="10"/>
+      <c r="DO16" s="10"/>
+      <c r="DQ16" s="14"/>
+      <c r="DR16" s="8"/>
+      <c r="DS16" s="8"/>
+      <c r="DT16" s="8"/>
+      <c r="DU16" s="8"/>
+      <c r="ED16" s="10"/>
+      <c r="EE16" s="10"/>
+      <c r="EF16" s="10"/>
+      <c r="EH16" s="14"/>
+      <c r="EI16" s="8"/>
+      <c r="EJ16" s="8"/>
+      <c r="EK16" s="8"/>
+      <c r="EL16" s="8"/>
+      <c r="EU16" s="10"/>
+      <c r="EV16" s="10"/>
+      <c r="EW16" s="10"/>
+      <c r="EY16" s="14"/>
+      <c r="EZ16" s="8"/>
+      <c r="FA16" s="8"/>
+      <c r="FB16" s="8"/>
+      <c r="FC16" s="8"/>
+      <c r="FL16" s="10"/>
+      <c r="FM16" s="10"/>
+      <c r="FN16" s="10"/>
+      <c r="FP16" s="14"/>
+      <c r="FQ16" s="8"/>
+      <c r="FR16" s="8"/>
+      <c r="FS16" s="8"/>
+      <c r="FT16" s="8"/>
+      <c r="GC16" s="10"/>
+      <c r="GD16" s="10"/>
+      <c r="GE16" s="10"/>
+      <c r="GG16" s="14"/>
+      <c r="GH16" s="8"/>
+      <c r="GI16" s="8"/>
+      <c r="GJ16" s="8"/>
+      <c r="GK16" s="8"/>
+      <c r="GT16" s="10"/>
+      <c r="GU16" s="10"/>
+      <c r="GV16" s="10"/>
+      <c r="GX16" s="14"/>
+      <c r="GY16" s="8"/>
+      <c r="GZ16" s="8"/>
+      <c r="HA16" s="8"/>
+      <c r="HB16" s="8"/>
+      <c r="HK16" s="10"/>
+      <c r="HL16" s="10"/>
+      <c r="HM16" s="10"/>
+      <c r="HO16" s="14"/>
+      <c r="HP16" s="8"/>
+      <c r="HQ16" s="8"/>
+      <c r="HR16" s="8"/>
+      <c r="HS16" s="8"/>
+      <c r="IB16" s="10"/>
+      <c r="IC16" s="10"/>
+      <c r="ID16" s="10"/>
+      <c r="IF16" s="14"/>
+      <c r="IG16" s="8"/>
+      <c r="IH16" s="8"/>
+      <c r="II16" s="8"/>
+      <c r="IJ16" s="8"/>
+      <c r="IS16" s="10"/>
+      <c r="IT16" s="10"/>
+      <c r="IU16" s="10"/>
+      <c r="IW16" s="14"/>
+      <c r="IX16" s="8"/>
+      <c r="IY16" s="8"/>
+      <c r="IZ16" s="8"/>
+      <c r="JA16" s="8"/>
+      <c r="JJ16" s="10"/>
+      <c r="JK16" s="10"/>
+      <c r="JL16" s="10"/>
+      <c r="JN16" s="14"/>
+      <c r="JO16" s="8"/>
+      <c r="JP16" s="8"/>
+      <c r="JQ16" s="8"/>
+      <c r="JR16" s="8"/>
+      <c r="KA16" s="10"/>
+      <c r="KB16" s="10"/>
+      <c r="KC16" s="10"/>
+      <c r="KE16" s="14"/>
+      <c r="KF16" s="8"/>
+      <c r="KG16" s="8"/>
+      <c r="KH16" s="8"/>
+      <c r="KI16" s="8"/>
+      <c r="KR16" s="10"/>
+      <c r="KS16" s="10"/>
+      <c r="KT16" s="10"/>
+      <c r="KV16" s="14"/>
+      <c r="KW16" s="8"/>
+      <c r="KX16" s="8"/>
+      <c r="KY16" s="8"/>
+      <c r="KZ16" s="8"/>
+      <c r="LI16" s="10"/>
+      <c r="LJ16" s="10"/>
+      <c r="LK16" s="10"/>
+      <c r="LM16" s="14"/>
+      <c r="LN16" s="8"/>
+      <c r="LO16" s="8"/>
+      <c r="LP16" s="8"/>
+      <c r="LQ16" s="8"/>
+      <c r="LZ16" s="10"/>
+      <c r="MA16" s="10"/>
+      <c r="MB16" s="10"/>
+      <c r="MD16" s="14"/>
+      <c r="ME16" s="8"/>
+      <c r="MF16" s="8"/>
+      <c r="MG16" s="8"/>
+      <c r="MH16" s="8"/>
+      <c r="MQ16" s="10"/>
+      <c r="MR16" s="10"/>
+      <c r="MS16" s="10"/>
+      <c r="MU16" s="14"/>
+      <c r="MV16" s="8"/>
+      <c r="MW16" s="8"/>
+      <c r="MX16" s="8"/>
+      <c r="MY16" s="8"/>
+      <c r="NH16" s="10"/>
+      <c r="NI16" s="10"/>
+      <c r="NJ16" s="10"/>
+      <c r="NL16" s="14"/>
+      <c r="NM16" s="8"/>
+      <c r="NN16" s="8"/>
+      <c r="NO16" s="8"/>
+      <c r="NP16" s="8"/>
+      <c r="NY16" s="10"/>
+      <c r="NZ16" s="10"/>
+      <c r="OA16" s="10"/>
+      <c r="OC16" s="14"/>
+      <c r="OD16" s="8"/>
+      <c r="OE16" s="8"/>
+      <c r="OF16" s="8"/>
+      <c r="OG16" s="8"/>
+      <c r="OP16" s="10"/>
+      <c r="OQ16" s="10"/>
+      <c r="OR16" s="10"/>
+      <c r="OT16" s="14"/>
+      <c r="OU16" s="8"/>
+      <c r="OV16" s="8"/>
+      <c r="OW16" s="8"/>
+      <c r="OX16" s="8"/>
+      <c r="PG16" s="10"/>
+      <c r="PH16" s="10"/>
+      <c r="PI16" s="10"/>
+      <c r="PK16" s="14"/>
+      <c r="PL16" s="8"/>
+      <c r="PM16" s="8"/>
+      <c r="PN16" s="8"/>
+      <c r="PO16" s="8"/>
+      <c r="PX16" s="10"/>
+      <c r="PY16" s="10"/>
+      <c r="PZ16" s="10"/>
+      <c r="QB16" s="14"/>
+      <c r="QC16" s="8"/>
+      <c r="QD16" s="8"/>
+      <c r="QE16" s="8"/>
+      <c r="QF16" s="8"/>
+      <c r="QO16" s="10"/>
+      <c r="QP16" s="10"/>
+      <c r="QQ16" s="10"/>
+      <c r="QS16" s="14"/>
+      <c r="QT16" s="8"/>
+      <c r="QU16" s="8"/>
+      <c r="QV16" s="8"/>
+      <c r="QW16" s="8"/>
+      <c r="RF16" s="10"/>
+      <c r="RG16" s="10"/>
+      <c r="RH16" s="10"/>
+      <c r="RJ16" s="14"/>
+      <c r="RK16" s="8"/>
+      <c r="RL16" s="8"/>
+      <c r="RM16" s="8"/>
+      <c r="RN16" s="8"/>
+      <c r="RW16" s="10"/>
+      <c r="RX16" s="10"/>
+      <c r="RY16" s="10"/>
+      <c r="SA16" s="14"/>
+      <c r="SB16" s="8"/>
+      <c r="SC16" s="8"/>
+      <c r="SD16" s="8"/>
+      <c r="SE16" s="8"/>
+      <c r="SN16" s="10"/>
+      <c r="SO16" s="10"/>
+      <c r="SP16" s="10"/>
+      <c r="SR16" s="14"/>
+      <c r="SS16" s="8"/>
+      <c r="ST16" s="8"/>
+      <c r="SU16" s="8"/>
+      <c r="SV16" s="8"/>
+      <c r="TE16" s="10"/>
+      <c r="TF16" s="10"/>
+      <c r="TG16" s="10"/>
+      <c r="TI16" s="14"/>
+      <c r="TJ16" s="8"/>
+      <c r="TK16" s="8"/>
+      <c r="TL16" s="8"/>
+      <c r="TM16" s="8"/>
+      <c r="TV16" s="10"/>
+      <c r="TW16" s="10"/>
+      <c r="TX16" s="10"/>
+      <c r="TZ16" s="14"/>
+      <c r="UA16" s="8"/>
+      <c r="UB16" s="8"/>
+      <c r="UC16" s="8"/>
+      <c r="UD16" s="8"/>
+      <c r="UM16" s="10"/>
+      <c r="UN16" s="10"/>
+      <c r="UO16" s="10"/>
+      <c r="UQ16" s="14"/>
+      <c r="UR16" s="8"/>
+      <c r="US16" s="8"/>
+      <c r="UT16" s="8"/>
+      <c r="UU16" s="8"/>
+      <c r="VD16" s="10"/>
+      <c r="VE16" s="10"/>
+      <c r="VF16" s="10"/>
+      <c r="VH16" s="14"/>
+      <c r="VI16" s="8"/>
+      <c r="VJ16" s="8"/>
+      <c r="VK16" s="8"/>
+      <c r="VL16" s="8"/>
+      <c r="VU16" s="10"/>
+      <c r="VV16" s="10"/>
+      <c r="VW16" s="10"/>
+      <c r="VY16" s="14"/>
+      <c r="VZ16" s="8"/>
+      <c r="WA16" s="8"/>
+      <c r="WB16" s="8"/>
+      <c r="WC16" s="8"/>
+      <c r="WL16" s="10"/>
+      <c r="WM16" s="10"/>
+      <c r="WN16" s="10"/>
+      <c r="WP16" s="14"/>
+      <c r="WQ16" s="8"/>
+      <c r="WR16" s="8"/>
+      <c r="WS16" s="8"/>
+      <c r="WT16" s="8"/>
+      <c r="XC16" s="10"/>
+      <c r="XD16" s="10"/>
+      <c r="XE16" s="10"/>
+      <c r="XG16" s="14"/>
+      <c r="XH16" s="8"/>
+      <c r="XI16" s="8"/>
+      <c r="XJ16" s="8"/>
+      <c r="XK16" s="8"/>
+      <c r="XT16" s="10"/>
+      <c r="XU16" s="10"/>
+      <c r="XV16" s="10"/>
+      <c r="XX16" s="14"/>
+      <c r="XY16" s="8"/>
+      <c r="XZ16" s="8"/>
+      <c r="YA16" s="8"/>
+      <c r="YB16" s="8"/>
+      <c r="YK16" s="10"/>
+      <c r="YL16" s="10"/>
+      <c r="YM16" s="10"/>
+      <c r="YO16" s="14"/>
+      <c r="YP16" s="8"/>
+      <c r="YQ16" s="8"/>
+      <c r="YR16" s="8"/>
+      <c r="YS16" s="8"/>
+      <c r="ZB16" s="10"/>
+      <c r="ZC16" s="10"/>
+      <c r="ZD16" s="10"/>
+      <c r="ZF16" s="14"/>
+      <c r="ZG16" s="8"/>
+      <c r="ZH16" s="8"/>
+      <c r="ZI16" s="8"/>
+      <c r="ZJ16" s="8"/>
+      <c r="ZS16" s="10"/>
+      <c r="ZT16" s="10"/>
+      <c r="ZU16" s="10"/>
+      <c r="ZW16" s="14"/>
+      <c r="ZX16" s="8"/>
+      <c r="ZY16" s="8"/>
+      <c r="ZZ16" s="8"/>
+      <c r="AAA16" s="8"/>
+      <c r="AAJ16" s="10"/>
+      <c r="AAK16" s="10"/>
+      <c r="AAL16" s="10"/>
+      <c r="AAN16" s="14"/>
+      <c r="AAO16" s="8"/>
+      <c r="AAP16" s="8"/>
+      <c r="AAQ16" s="8"/>
+      <c r="AAR16" s="8"/>
+      <c r="ABA16" s="10"/>
+      <c r="ABB16" s="10"/>
+      <c r="ABC16" s="10"/>
+      <c r="ABE16" s="14"/>
+      <c r="ABF16" s="8"/>
+      <c r="ABG16" s="8"/>
+      <c r="ABH16" s="8"/>
+      <c r="ABI16" s="8"/>
+      <c r="ABR16" s="10"/>
+      <c r="ABS16" s="10"/>
+      <c r="ABT16" s="10"/>
+      <c r="ABV16" s="14"/>
+      <c r="ABW16" s="8"/>
+      <c r="ABX16" s="8"/>
+      <c r="ABY16" s="8"/>
+      <c r="ABZ16" s="8"/>
+      <c r="ACI16" s="10"/>
+      <c r="ACJ16" s="10"/>
+      <c r="ACK16" s="10"/>
+      <c r="ACM16" s="14"/>
+      <c r="ACN16" s="8"/>
+      <c r="ACO16" s="8"/>
+      <c r="ACP16" s="8"/>
+      <c r="ACQ16" s="8"/>
+      <c r="ACZ16" s="10"/>
+      <c r="ADA16" s="10"/>
+      <c r="ADB16" s="10"/>
+      <c r="ADD16" s="14"/>
+      <c r="ADE16" s="8"/>
+      <c r="ADF16" s="8"/>
+      <c r="ADG16" s="8"/>
+      <c r="ADH16" s="8"/>
+      <c r="ADQ16" s="10"/>
+      <c r="ADR16" s="10"/>
+      <c r="ADS16" s="10"/>
+      <c r="ADU16" s="14"/>
+      <c r="ADV16" s="8"/>
+      <c r="ADW16" s="8"/>
+      <c r="ADX16" s="8"/>
+      <c r="ADY16" s="8"/>
+      <c r="AEH16" s="10"/>
+      <c r="AEI16" s="10"/>
+      <c r="AEJ16" s="10"/>
+      <c r="AEL16" s="14"/>
+      <c r="AEM16" s="8"/>
+      <c r="AEN16" s="8"/>
+      <c r="AEO16" s="8"/>
+      <c r="AEP16" s="8"/>
+      <c r="AEY16" s="10"/>
+      <c r="AEZ16" s="10"/>
+      <c r="AFA16" s="10"/>
+      <c r="AFC16" s="14"/>
+      <c r="AFD16" s="8"/>
+      <c r="AFE16" s="8"/>
+      <c r="AFF16" s="8"/>
+      <c r="AFG16" s="8"/>
+      <c r="AFP16" s="10"/>
+      <c r="AFQ16" s="10"/>
+      <c r="AFR16" s="10"/>
+      <c r="AFT16" s="14"/>
+      <c r="AFU16" s="8"/>
+      <c r="AFV16" s="8"/>
+      <c r="AFW16" s="8"/>
+      <c r="AFX16" s="8"/>
+      <c r="AGG16" s="10"/>
+      <c r="AGH16" s="10"/>
+      <c r="AGI16" s="10"/>
+      <c r="AGK16" s="14"/>
+      <c r="AGL16" s="8"/>
+      <c r="AGM16" s="8"/>
+      <c r="AGN16" s="8"/>
+      <c r="AGO16" s="8"/>
+      <c r="AGX16" s="10"/>
+      <c r="AGY16" s="10"/>
+      <c r="AGZ16" s="10"/>
+      <c r="AHB16" s="14"/>
+      <c r="AHC16" s="8"/>
+      <c r="AHD16" s="8"/>
+      <c r="AHE16" s="8"/>
+      <c r="AHF16" s="8"/>
+      <c r="AHO16" s="10"/>
+      <c r="AHP16" s="10"/>
+      <c r="AHQ16" s="10"/>
+      <c r="AHS16" s="14"/>
+      <c r="AHT16" s="8"/>
+      <c r="AHU16" s="8"/>
+      <c r="AHV16" s="8"/>
+      <c r="AHW16" s="8"/>
+      <c r="AIF16" s="10"/>
+      <c r="AIG16" s="10"/>
+      <c r="AIH16" s="10"/>
+      <c r="AIJ16" s="14"/>
+      <c r="AIK16" s="8"/>
+      <c r="AIL16" s="8"/>
+      <c r="AIM16" s="8"/>
+      <c r="AIN16" s="8"/>
+      <c r="AIW16" s="10"/>
+      <c r="AIX16" s="10"/>
+      <c r="AIY16" s="10"/>
+      <c r="AJA16" s="14"/>
+      <c r="AJB16" s="8"/>
+      <c r="AJC16" s="8"/>
+      <c r="AJD16" s="8"/>
+      <c r="AJE16" s="8"/>
+      <c r="AJN16" s="10"/>
+      <c r="AJO16" s="10"/>
+      <c r="AJP16" s="10"/>
+      <c r="AJR16" s="14"/>
+      <c r="AJS16" s="8"/>
+      <c r="AJT16" s="8"/>
+      <c r="AJU16" s="8"/>
+      <c r="AJV16" s="8"/>
+      <c r="AKE16" s="10"/>
+      <c r="AKF16" s="10"/>
+      <c r="AKG16" s="10"/>
+      <c r="AKI16" s="14"/>
+      <c r="AKJ16" s="8"/>
+      <c r="AKK16" s="8"/>
+      <c r="AKL16" s="8"/>
+      <c r="AKM16" s="8"/>
+      <c r="AKV16" s="10"/>
+      <c r="AKW16" s="10"/>
+      <c r="AKX16" s="10"/>
+      <c r="AKZ16" s="14"/>
+      <c r="ALA16" s="8"/>
+      <c r="ALB16" s="8"/>
+      <c r="ALC16" s="8"/>
+      <c r="ALD16" s="8"/>
+      <c r="ALM16" s="10"/>
+      <c r="ALN16" s="10"/>
+      <c r="ALO16" s="10"/>
+      <c r="ALQ16" s="14"/>
+      <c r="ALR16" s="8"/>
+      <c r="ALS16" s="8"/>
+      <c r="ALT16" s="8"/>
+      <c r="ALU16" s="8"/>
+      <c r="AMD16" s="10"/>
+      <c r="AME16" s="10"/>
+      <c r="AMF16" s="10"/>
+      <c r="AMH16" s="14"/>
+      <c r="AMI16" s="8"/>
+      <c r="AMJ16" s="8"/>
     </row>
     <row r="17" ht="31.5" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>123456</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="11">
         <v>1</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="11">
         <v>1</v>
       </c>
       <c r="L17" s="4" t="s">
@@ -2596,13 +2572,13 @@
       <c r="N17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O17" s="14">
+      <c r="O17" s="12">
         <v>45384</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="P17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R17" s="2">
@@ -2632,7 +2608,7 @@
       <c r="Z17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC17" s="5">
+      <c r="AC17" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -2640,13 +2616,13 @@
       <c r="A18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="15">
         <v>123456</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -2655,19 +2631,19 @@
       <c r="F18" s="3">
         <v>123456</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="13" t="s">
+      <c r="J18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L18" s="4" t="s">
@@ -2715,7 +2691,7 @@
       <c r="Z18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC18" s="5">
+      <c r="AC18" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -2723,25 +2699,25 @@
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>123456</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="10">
-        <v>123456</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="8">
+        <v>123456</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2762,11 +2738,11 @@
       <c r="N19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12" t="s">
+      <c r="O19" s="10"/>
+      <c r="P19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q19" s="12" t="s">
+      <c r="Q19" s="10" t="s">
         <v>45</v>
       </c>
       <c r="R19" s="4" t="s">
@@ -2793,7 +2769,7 @@
       <c r="Z19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC19" s="5">
+      <c r="AC19" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -2801,7 +2777,7 @@
       <c r="A20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -2816,19 +2792,19 @@
       <c r="F20" s="3">
         <v>123456</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="13" t="s">
+      <c r="J20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L20" s="4" t="s">
@@ -2876,7 +2852,7 @@
       <c r="Z20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC20" s="5">
+      <c r="AC20" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -2884,7 +2860,7 @@
       <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2899,19 +2875,19 @@
       <c r="F21" s="3">
         <v>123456</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K21" s="13" t="s">
+      <c r="J21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L21" s="4" t="s">
@@ -2923,7 +2899,7 @@
       <c r="N21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O21" s="18">
+      <c r="O21" s="16">
         <v>45384</v>
       </c>
       <c r="P21" s="3" t="s">
@@ -2959,7 +2935,7 @@
       <c r="Z21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC21" s="5">
+      <c r="AC21" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -2967,34 +2943,34 @@
       <c r="A22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>123456</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="F22" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="11">
         <v>1</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="11">
         <v>1</v>
       </c>
       <c r="L22" s="4" t="s">
@@ -3006,13 +2982,13 @@
       <c r="N22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="14">
+      <c r="O22" s="12">
         <v>45384</v>
       </c>
-      <c r="P22" s="14" t="s">
+      <c r="P22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q22" s="14" t="s">
+      <c r="Q22" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R22" s="2">
@@ -3042,7 +3018,7 @@
       <c r="Z22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AC22" s="5">
+      <c r="AC22" s="3">
         <v>9874563212</v>
       </c>
     </row>
@@ -3050,34 +3026,34 @@
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>123456</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="F23" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="11">
         <v>1</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="11">
         <v>1</v>
       </c>
       <c r="L23" s="4" t="s">
@@ -3089,13 +3065,13 @@
       <c r="N23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O23" s="14">
+      <c r="O23" s="12">
         <v>45384</v>
       </c>
-      <c r="P23" s="14" t="s">
+      <c r="P23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q23" s="14" t="s">
+      <c r="Q23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R23" s="2">
@@ -3125,42 +3101,42 @@
       <c r="Z23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AC23" s="5">
+      <c r="AC23" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="14.25">
       <c r="A24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>123456</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="11">
         <v>1</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="11">
         <v>1</v>
       </c>
       <c r="L24" s="4" t="s">
@@ -3172,13 +3148,13 @@
       <c r="N24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O24" s="14">
+      <c r="O24" s="12">
         <v>45384</v>
       </c>
-      <c r="P24" s="14" t="s">
+      <c r="P24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q24" s="14" t="s">
+      <c r="Q24" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R24" s="2">
@@ -3208,42 +3184,42 @@
       <c r="Z24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC24" s="5">
+      <c r="AC24" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="14.25">
       <c r="A25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>123456</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G25" s="8" t="s">
+      <c r="F25" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="11">
         <v>1</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="11">
         <v>1</v>
       </c>
       <c r="L25" s="4" t="s">
@@ -3255,13 +3231,13 @@
       <c r="N25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O25" s="14">
+      <c r="O25" s="12">
         <v>45384</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="P25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q25" s="14" t="s">
+      <c r="Q25" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R25" s="2">
@@ -3294,42 +3270,42 @@
       <c r="AB25" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AC25" s="5">
+      <c r="AC25" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="14.25">
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>123456</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G26" s="8" t="s">
+      <c r="F26" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="11">
         <v>1</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="11">
         <v>1</v>
       </c>
       <c r="L26" s="4" t="s">
@@ -3341,13 +3317,13 @@
       <c r="N26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O26" s="14">
+      <c r="O26" s="12">
         <v>45384</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="P26" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q26" s="14" t="s">
+      <c r="Q26" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R26" s="2">
@@ -3377,42 +3353,42 @@
       <c r="Z26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC26" s="5">
+      <c r="AC26" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="14.25">
       <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>123456</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G27" s="8" t="s">
+      <c r="F27" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="11">
         <v>1</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="11">
         <v>1</v>
       </c>
       <c r="L27" s="4" t="s">
@@ -3424,13 +3400,13 @@
       <c r="N27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O27" s="14">
+      <c r="O27" s="12">
         <v>45384</v>
       </c>
-      <c r="P27" s="14" t="s">
+      <c r="P27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q27" s="14" t="s">
+      <c r="Q27" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R27" s="2">
@@ -3460,42 +3436,42 @@
       <c r="Z27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC27" s="5">
+      <c r="AC27" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="14.25">
       <c r="A28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="6">
-        <v>123456</v>
-      </c>
-      <c r="E28" s="17" t="s">
+      <c r="D28" s="5">
+        <v>123456</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G28" s="8" t="s">
+      <c r="F28" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="11">
         <v>1</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="11">
         <v>1</v>
       </c>
       <c r="L28" s="4" t="s">
@@ -3507,13 +3483,13 @@
       <c r="N28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O28" s="14">
+      <c r="O28" s="12">
         <v>45384</v>
       </c>
-      <c r="P28" s="14" t="s">
+      <c r="P28" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q28" s="14" t="s">
+      <c r="Q28" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R28" s="2">
@@ -3543,42 +3519,42 @@
       <c r="Z28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC28" s="5">
+      <c r="AC28" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" ht="14.25">
       <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>123456</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G29" s="8" t="s">
+      <c r="F29" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="11">
         <v>1</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="11">
         <v>1</v>
       </c>
       <c r="L29" s="4" t="s">
@@ -3590,13 +3566,13 @@
       <c r="N29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O29" s="14">
+      <c r="O29" s="12">
         <v>45384</v>
       </c>
-      <c r="P29" s="14" t="s">
+      <c r="P29" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q29" s="14" t="s">
+      <c r="Q29" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R29" s="2">
@@ -3626,42 +3602,42 @@
       <c r="Z29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC29" s="5">
+      <c r="AC29" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="14.25">
       <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>123456</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G30" s="8" t="s">
+      <c r="F30" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="11">
         <v>1</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="11">
         <v>1</v>
       </c>
       <c r="L30" s="4" t="s">
@@ -3673,13 +3649,13 @@
       <c r="N30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O30" s="14">
+      <c r="O30" s="12">
         <v>45384</v>
       </c>
-      <c r="P30" s="14" t="s">
+      <c r="P30" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q30" s="14" t="s">
+      <c r="Q30" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R30" s="2">
@@ -3709,36 +3685,36 @@
       <c r="Z30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC30" s="5">
+      <c r="AC30" s="3">
         <v>9874563212</v>
       </c>
     </row>
     <row r="31" ht="25.5">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>123456</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="9">
-        <v>123456</v>
-      </c>
-      <c r="G31" s="8" t="s">
+      <c r="F31" s="7">
+        <v>123456</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J31" s="1" t="s">
@@ -3750,17 +3726,17 @@
       <c r="L31" s="1">
         <v>2</v>
       </c>
-      <c r="M31" s="9" t="s">
+      <c r="M31" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="N31" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O31" s="12"/>
-      <c r="P31" s="9" t="s">
+      <c r="O31" s="10"/>
+      <c r="P31" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Q31" s="9" t="s">
+      <c r="Q31" s="7" t="s">
         <v>45</v>
       </c>
       <c r="R31" s="2">
@@ -3790,15 +3766,15 @@
       <c r="Z31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC31" s="5">
+      <c r="AC31" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" ht="14.25">
       <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -3813,19 +3789,19 @@
       <c r="F32" s="3">
         <v>123456</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K32" s="13" t="s">
+      <c r="J32" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K32" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="4" t="s">
@@ -3837,7 +3813,7 @@
       <c r="N32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O32" s="18">
+      <c r="O32" s="16">
         <v>45384</v>
       </c>
       <c r="P32" s="3" t="s">
@@ -3873,42 +3849,42 @@
       <c r="Z32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC32" s="5">
+      <c r="AC32" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" ht="14.25">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>123456</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G33" s="8" t="s">
+      <c r="F33" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="11">
         <v>1</v>
       </c>
-      <c r="K33" s="13">
+      <c r="K33" s="11">
         <v>1</v>
       </c>
       <c r="L33" s="4" t="s">
@@ -3920,13 +3896,13 @@
       <c r="N33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O33" s="14">
+      <c r="O33" s="12">
         <v>45384</v>
       </c>
-      <c r="P33" s="14" t="s">
+      <c r="P33" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q33" s="14" t="s">
+      <c r="Q33" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R33" s="2">
@@ -3956,125 +3932,125 @@
       <c r="Z33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC33" s="5">
+      <c r="AC33" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="34" s="2" customFormat="1">
+    <row r="34" s="2" customFormat="1" ht="14.25">
       <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="17">
         <v>123456</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="19">
-        <v>123456</v>
-      </c>
-      <c r="G34" s="8" t="s">
+      <c r="F34" s="17">
+        <v>123456</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="11">
         <v>1</v>
       </c>
-      <c r="K34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="M34" s="13" t="s">
+      <c r="K34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M34" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="O34" s="20">
+      <c r="N34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O34" s="18">
         <v>45384</v>
       </c>
-      <c r="P34" s="21" t="s">
+      <c r="P34" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="Q34" s="21" t="s">
+      <c r="Q34" s="19" t="s">
         <v>45</v>
       </c>
       <c r="R34" s="2">
         <v>7709577438</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="S34" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="T34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="U34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="W34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="X34" s="13" t="s">
+      <c r="T34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="U34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="V34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="W34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="X34" s="11" t="s">
         <v>36</v>
       </c>
       <c r="Y34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Z34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC34" s="5">
+      <c r="Z34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC34" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="14.25">
       <c r="A35" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>123456</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G35" s="8" t="s">
+      <c r="F35" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="11">
         <v>1</v>
       </c>
-      <c r="K35" s="13">
+      <c r="K35" s="11">
         <v>1</v>
       </c>
       <c r="L35" s="4" t="s">
@@ -4086,13 +4062,13 @@
       <c r="N35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O35" s="14">
+      <c r="O35" s="12">
         <v>45384</v>
       </c>
-      <c r="P35" s="14" t="s">
+      <c r="P35" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q35" s="14" t="s">
+      <c r="Q35" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R35" s="2">
@@ -4122,42 +4098,42 @@
       <c r="Z35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AC35" s="5">
+      <c r="AC35" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="14.25">
       <c r="A36" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>123456</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="6">
-        <v>123456</v>
-      </c>
-      <c r="G36" s="8" t="s">
+      <c r="F36" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K36" s="13" t="s">
+      <c r="J36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K36" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L36" s="4" t="s">
@@ -4169,13 +4145,13 @@
       <c r="N36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O36" s="14">
+      <c r="O36" s="12">
         <v>45384</v>
       </c>
-      <c r="P36" s="14" t="s">
+      <c r="P36" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q36" s="14" t="s">
+      <c r="Q36" s="12" t="s">
         <v>45</v>
       </c>
       <c r="R36" s="2">
@@ -4205,15 +4181,15 @@
       <c r="Z36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC36" s="5">
+      <c r="AC36" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="14.25">
       <c r="A37" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -4228,19 +4204,19 @@
       <c r="F37" s="3">
         <v>123456</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K37" s="13" t="s">
+      <c r="J37" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L37" s="4" t="s">
@@ -4252,7 +4228,7 @@
       <c r="N37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O37" s="18">
+      <c r="O37" s="16">
         <v>45384</v>
       </c>
       <c r="P37" s="3" t="s">
@@ -4288,15 +4264,15 @@
       <c r="Z37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC37" s="5">
+      <c r="AC37" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="14.25">
       <c r="A38" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -4311,19 +4287,19 @@
       <c r="F38" s="3">
         <v>123456</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J38" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K38" s="13" t="s">
+      <c r="J38" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L38" s="4" t="s">
@@ -4335,7 +4311,7 @@
       <c r="N38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O38" s="18">
+      <c r="O38" s="16">
         <v>45384</v>
       </c>
       <c r="P38" s="3" t="s">
@@ -4371,36 +4347,36 @@
       <c r="Z38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC38" s="5">
+      <c r="AC38" s="3">
         <v>9874563212</v>
       </c>
     </row>
     <row r="39" ht="25.5">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="7">
         <v>123456</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="9">
-        <v>123456</v>
-      </c>
-      <c r="G39" s="8" t="s">
+      <c r="F39" s="7">
+        <v>123456</v>
+      </c>
+      <c r="G39" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J39" s="1" t="s">
@@ -4412,19 +4388,19 @@
       <c r="L39" s="1">
         <v>2</v>
       </c>
-      <c r="M39" s="9" t="s">
+      <c r="M39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N39" s="9" t="s">
+      <c r="N39" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O39" s="18">
+      <c r="O39" s="16">
         <v>45384</v>
       </c>
-      <c r="P39" s="9" t="s">
+      <c r="P39" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Q39" s="9" t="s">
+      <c r="Q39" s="7" t="s">
         <v>45</v>
       </c>
       <c r="R39" s="4" t="s">
@@ -4455,36 +4431,36 @@
         <v>36</v>
       </c>
       <c r="AA39" s="4"/>
-      <c r="AC39" s="5">
+      <c r="AC39" s="3">
         <v>9874563212</v>
       </c>
     </row>
     <row r="40" ht="25.5">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="7">
         <v>123456</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="9">
-        <v>123456</v>
-      </c>
-      <c r="G40" s="8" t="s">
+      <c r="F40" s="7">
+        <v>123456</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="I40" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J40" s="1" t="s">
@@ -4496,19 +4472,19 @@
       <c r="L40" s="1">
         <v>2</v>
       </c>
-      <c r="M40" s="9" t="s">
+      <c r="M40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N40" s="9" t="s">
+      <c r="N40" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O40" s="18">
+      <c r="O40" s="16">
         <v>45384</v>
       </c>
-      <c r="P40" s="9" t="s">
+      <c r="P40" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Q40" s="9" t="s">
+      <c r="Q40" s="7" t="s">
         <v>45</v>
       </c>
       <c r="R40" s="4" t="s">
@@ -4539,36 +4515,36 @@
         <v>36</v>
       </c>
       <c r="AA40" s="4"/>
-      <c r="AC40" s="5">
+      <c r="AC40" s="3">
         <v>9874563212</v>
       </c>
     </row>
     <row r="41" ht="25.5">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="7">
         <v>123456</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="9">
-        <v>123456</v>
-      </c>
-      <c r="G41" s="8" t="s">
+      <c r="F41" s="7">
+        <v>123456</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="I41" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -4580,19 +4556,19 @@
       <c r="L41" s="1">
         <v>2</v>
       </c>
-      <c r="M41" s="9" t="s">
+      <c r="M41" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N41" s="9" t="s">
+      <c r="N41" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O41" s="18">
+      <c r="O41" s="16">
         <v>45384</v>
       </c>
-      <c r="P41" s="9" t="s">
+      <c r="P41" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="Q41" s="9" t="s">
+      <c r="Q41" s="7" t="s">
         <v>45</v>
       </c>
       <c r="R41" s="4" t="s">
@@ -4623,15 +4599,15 @@
         <v>36</v>
       </c>
       <c r="AA41" s="4"/>
-      <c r="AC41" s="5">
+      <c r="AC41" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" ht="14.25">
       <c r="A42" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -4646,31 +4622,31 @@
       <c r="F42" s="3">
         <v>123456</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K42" s="13" t="s">
+      <c r="J42" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M42" s="9" t="s">
+      <c r="M42" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="N42" s="9" t="s">
+      <c r="N42" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="O42" s="18">
+      <c r="O42" s="16">
         <v>45384</v>
       </c>
       <c r="P42" s="3" t="s">
@@ -4703,15 +4679,15 @@
       <c r="Z42" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC42" s="5">
+      <c r="AC42" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" ht="14.25">
       <c r="A43" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -4726,19 +4702,19 @@
       <c r="F43" s="3">
         <v>123456</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J43" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K43" s="13" t="s">
+      <c r="J43" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K43" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L43" s="4" t="s">
@@ -4783,15 +4759,15 @@
       <c r="Z43" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC43" s="5">
+      <c r="AC43" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="14.25">
       <c r="A44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -4806,19 +4782,19 @@
       <c r="F44" s="3">
         <v>123456</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K44" s="13" t="s">
+      <c r="J44" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K44" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L44" s="4" t="s">
@@ -4863,15 +4839,15 @@
       <c r="Z44" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC44" s="5">
+      <c r="AC44" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="14.25">
       <c r="A45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -4886,19 +4862,19 @@
       <c r="F45" s="3">
         <v>123456</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J45" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K45" s="13" t="s">
+      <c r="J45" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K45" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L45" s="4" t="s">
@@ -4943,15 +4919,15 @@
       <c r="Z45" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC45" s="5">
+      <c r="AC45" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" ht="14.25">
       <c r="A46" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -4966,19 +4942,19 @@
       <c r="F46" s="3">
         <v>123456</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J46" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K46" s="13" t="s">
+      <c r="J46" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K46" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L46" s="4" t="s">
@@ -5023,15 +4999,15 @@
       <c r="Z46" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC46" s="5">
+      <c r="AC46" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" ht="14.25">
       <c r="A47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -5046,19 +5022,19 @@
       <c r="F47" s="3">
         <v>123456</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J47" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K47" s="13" t="s">
+      <c r="J47" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K47" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L47" s="4" t="s">
@@ -5103,15 +5079,15 @@
       <c r="Z47" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC47" s="5">
+      <c r="AC47" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="14.25">
       <c r="A48" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -5126,19 +5102,19 @@
       <c r="F48" s="3">
         <v>123456</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J48" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K48" s="13" t="s">
+      <c r="J48" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K48" s="11" t="s">
         <v>36</v>
       </c>
       <c r="L48" s="4" t="s">
@@ -5183,15 +5159,15 @@
       <c r="Z48" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC48" s="5">
+      <c r="AC48" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" ht="14.25">
       <c r="A49" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -5206,10 +5182,10 @@
       <c r="F49" s="3">
         <v>123456</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I49" s="3" t="s">
@@ -5263,15 +5239,15 @@
       <c r="Z49" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC49" s="5">
+      <c r="AC49" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="14.25">
       <c r="A50" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -5286,10 +5262,10 @@
       <c r="F50" s="3">
         <v>123456</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="H50" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I50" s="3" t="s">
@@ -5343,15 +5319,15 @@
       <c r="Z50" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC50" s="5">
+      <c r="AC50" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" ht="14.25">
       <c r="A51" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -5366,10 +5342,10 @@
       <c r="F51" s="3">
         <v>123456</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I51" s="3" t="s">
@@ -5423,15 +5399,15 @@
       <c r="Z51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC51" s="5">
+      <c r="AC51" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" ht="14.25">
       <c r="A52" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -5446,10 +5422,10 @@
       <c r="F52" s="3">
         <v>123456</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I52" s="3" t="s">
@@ -5503,15 +5479,15 @@
       <c r="Z52" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC52" s="5">
+      <c r="AC52" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" ht="14.25">
       <c r="A53" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -5526,10 +5502,10 @@
       <c r="F53" s="3">
         <v>123456</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I53" s="3" t="s">
@@ -5583,15 +5559,15 @@
       <c r="Z53" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC53" s="5">
+      <c r="AC53" s="3">
         <v>9874563212</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" ht="14.25">
       <c r="A54" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>120</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -5606,10 +5582,10 @@
       <c r="F54" s="3">
         <v>123456</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="H54" s="6" t="s">
         <v>34</v>
       </c>
       <c r="I54" s="3" t="s">
@@ -5663,193 +5639,193 @@
       <c r="Z54" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC54" s="5">
+      <c r="AC54" s="3">
         <v>9874563214</v>
       </c>
     </row>
-    <row r="55">
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="F55" s="6"/>
+    <row r="55" ht="14.25">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="I55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
       <c r="R55" s="2"/>
       <c r="Z55" s="4"/>
-      <c r="AC55" s="5"/>
-    </row>
-    <row r="56">
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="AC55" s="3"/>
+    </row>
+    <row r="56" ht="14.25">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="F56" s="5"/>
       <c r="I56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
-      <c r="O56" s="14"/>
-      <c r="P56" s="14"/>
-      <c r="Q56" s="14"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
       <c r="R56" s="2"/>
       <c r="Z56" s="4"/>
-      <c r="AC56" s="5"/>
-    </row>
-    <row r="57">
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="AC56" s="3"/>
+    </row>
+    <row r="57" ht="14.25">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="F57" s="5"/>
       <c r="I57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
       <c r="R57" s="2"/>
-      <c r="AC57" s="5"/>
-    </row>
-    <row r="58">
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="AC57" s="3"/>
+    </row>
+    <row r="58" ht="14.25">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="F58" s="5"/>
       <c r="I58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
-      <c r="O58" s="14"/>
-      <c r="P58" s="14"/>
-      <c r="Q58" s="14"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
       <c r="R58" s="2"/>
-      <c r="AC58" s="5"/>
-    </row>
-    <row r="59">
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="F59" s="6"/>
+      <c r="AC58" s="3"/>
+    </row>
+    <row r="59" ht="14.25">
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="F59" s="5"/>
       <c r="I59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="14"/>
-      <c r="Q59" s="14"/>
+      <c r="O59" s="12"/>
+      <c r="P59" s="12"/>
+      <c r="Q59" s="12"/>
       <c r="R59" s="2"/>
-      <c r="AC59" s="5"/>
-    </row>
-    <row r="60">
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="AC59" s="3"/>
+    </row>
+    <row r="60" ht="14.25">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="F60" s="5"/>
       <c r="I60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
-      <c r="O60" s="14"/>
-      <c r="P60" s="14"/>
-      <c r="Q60" s="14"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
       <c r="R60" s="2"/>
-      <c r="AC60" s="5"/>
-    </row>
-    <row r="61">
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="AC60" s="3"/>
+    </row>
+    <row r="61" ht="14.25">
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="F61" s="5"/>
       <c r="I61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
-      <c r="O61" s="14"/>
-      <c r="P61" s="14"/>
-      <c r="Q61" s="14"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12"/>
       <c r="R61" s="2"/>
-      <c r="AC61" s="5"/>
-    </row>
-    <row r="62">
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="F62" s="6"/>
+      <c r="AC61" s="3"/>
+    </row>
+    <row r="62" ht="14.25">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="F62" s="5"/>
       <c r="I62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
-      <c r="O62" s="14"/>
-      <c r="P62" s="14"/>
-      <c r="Q62" s="14"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
       <c r="R62" s="2"/>
-      <c r="AC62" s="5"/>
-    </row>
-    <row r="63">
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="AC62" s="3"/>
+    </row>
+    <row r="63" ht="14.25">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="F63" s="5"/>
       <c r="I63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
-      <c r="O63" s="14"/>
-      <c r="P63" s="14"/>
-      <c r="Q63" s="14"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12"/>
       <c r="R63" s="2"/>
-      <c r="AC63" s="5"/>
-    </row>
-    <row r="64">
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="F64" s="6"/>
+      <c r="AC63" s="3"/>
+    </row>
+    <row r="64" ht="14.25">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="F64" s="5"/>
       <c r="I64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
-      <c r="O64" s="14"/>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
       <c r="R64" s="2"/>
-      <c r="AC64" s="5"/>
-    </row>
-    <row r="65">
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="F65" s="6"/>
+      <c r="AC64" s="3"/>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="F65" s="5"/>
       <c r="I65" s="4"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
-      <c r="O65" s="14"/>
-      <c r="P65" s="14"/>
-      <c r="Q65" s="14"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12"/>
       <c r="R65" s="2"/>
-      <c r="AC65" s="5"/>
-    </row>
-    <row r="66">
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="AC65" s="3"/>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="F66" s="5"/>
       <c r="I66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
-      <c r="O66" s="14"/>
-      <c r="P66" s="14"/>
-      <c r="Q66" s="14"/>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12"/>
       <c r="R66" s="2"/>
-      <c r="AC66" s="5"/>
-    </row>
-    <row r="67">
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="F67" s="6"/>
+      <c r="AC66" s="3"/>
+    </row>
+    <row r="67" ht="14.25">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="F67" s="5"/>
       <c r="I67" s="4"/>
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
-      <c r="O67" s="14"/>
-      <c r="P67" s="14"/>
-      <c r="Q67" s="14"/>
+      <c r="O67" s="12"/>
+      <c r="P67" s="12"/>
+      <c r="Q67" s="12"/>
       <c r="R67" s="2"/>
-      <c r="AC67" s="5"/>
+      <c r="AC67" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>